<commit_message>
attempt of lumping loop failed
error when performing the II cycle when fitting, still obscure
</commit_message>
<xml_diff>
--- a/C5H5OH/clock_Pi.xlsx
+++ b/C5H5OH/clock_Pi.xlsx
@@ -388,13 +388,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3473058999999985</v>
+        <v>0.2590806999999984</v>
       </c>
       <c r="C2" t="n">
-        <v>22.7149349</v>
+        <v>18.928215</v>
       </c>
       <c r="D2" t="n">
-        <v>4.736604300000003</v>
+        <v>3.776661900000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>